<commit_message>
Add header of table
</commit_message>
<xml_diff>
--- a/Error_KCube_read.xlsx
+++ b/Error_KCube_read.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\INTERNSHIP_PROGRAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A95B663-BFC3-4FF7-AAEF-24E091CA6FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C2DA8C-7F62-422A-9F3F-41FCD855E56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{26BB2A2F-5459-461A-9D0C-B97101B86A4E}"/>
   </bookViews>
@@ -36,9 +36,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>error = 0.01 - 0.05</t>
+  </si>
+  <si>
+    <t>10mm</t>
+  </si>
+  <si>
+    <t>20mm</t>
+  </si>
+  <si>
+    <t>30mm</t>
+  </si>
+  <si>
+    <t>40 mm</t>
+  </si>
+  <si>
+    <t>50mm</t>
+  </si>
+  <si>
+    <t>60mm</t>
+  </si>
+  <si>
+    <t>70mm</t>
+  </si>
+  <si>
+    <t>90mm</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>#3</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>#7</t>
+  </si>
+  <si>
+    <t>#8</t>
+  </si>
+  <si>
+    <t>#9</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Calculated</t>
   </si>
 </sst>
 </file>
@@ -58,7 +115,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -77,6 +134,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -90,11 +159,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -103,6 +180,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF7C80"/>
+      <color rgb="FFFFCCCC"/>
       <color rgb="FFFFFFCC"/>
     </mruColors>
   </colors>
@@ -434,18 +513,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0D5208A-B13A-46AA-AC44-509BA473E653}">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="11" max="11" width="17.5" customWidth="1"/>
+    <col min="11" max="11" width="10.69921875" customWidth="1"/>
+    <col min="14" max="15" width="10.69921875" customWidth="1"/>
+    <col min="18" max="18" width="17.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A1">
         <v>70.007999999999996</v>
       </c>
@@ -456,7 +537,7 @@
         <v>70.010000000000005</v>
       </c>
       <c r="D1">
-        <f>SUM(A1:C1)</f>
+        <f t="shared" ref="D1:D9" si="0">SUM(A1:C1)</f>
         <v>210.02600000000001</v>
       </c>
       <c r="F1">
@@ -471,11 +552,8 @@
         <f>G1-F1</f>
         <v>-4.7500000000013642E-2</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>19.998999999999999</v>
       </c>
@@ -486,7 +564,7 @@
         <v>19.998999999999999</v>
       </c>
       <c r="D2">
-        <f>SUM(A2:C2)</f>
+        <f t="shared" si="0"/>
         <v>59.997</v>
       </c>
       <c r="F2">
@@ -498,11 +576,11 @@
         <v>180</v>
       </c>
       <c r="I2" s="2">
-        <f t="shared" ref="I2:I3" si="0">G2-F2</f>
+        <f t="shared" ref="I2:I3" si="1">G2-F2</f>
         <v>2.4499999999989086E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>50.006500000000003</v>
       </c>
@@ -513,7 +591,7 @@
         <v>50.009</v>
       </c>
       <c r="D3">
-        <f>SUM(A3:C3)</f>
+        <f t="shared" si="0"/>
         <v>150.02199999999999</v>
       </c>
       <c r="F3">
@@ -525,11 +603,11 @@
         <v>450</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-3.999999999996362E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>70.000500000000002</v>
       </c>
@@ -540,11 +618,11 @@
         <v>70.001000000000005</v>
       </c>
       <c r="D4">
-        <f>SUM(A4:C4)</f>
+        <f t="shared" si="0"/>
         <v>210.00250000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>19.994</v>
       </c>
@@ -555,11 +633,11 @@
         <v>19.998999999999999</v>
       </c>
       <c r="D5">
-        <f>SUM(A5:C5)</f>
+        <f t="shared" si="0"/>
         <v>59.986999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>50.000999999999998</v>
       </c>
@@ -570,11 +648,11 @@
         <v>50.0075</v>
       </c>
       <c r="D6">
-        <f>SUM(A6:C6)</f>
+        <f t="shared" si="0"/>
         <v>150.0095</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>70.009</v>
       </c>
@@ -585,11 +663,11 @@
         <v>70.001000000000005</v>
       </c>
       <c r="D7">
-        <f>SUM(A7:C7)</f>
+        <f t="shared" si="0"/>
         <v>210.01900000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>19.999500000000001</v>
       </c>
@@ -600,11 +678,11 @@
         <v>19.992999999999999</v>
       </c>
       <c r="D8">
-        <f>SUM(A8:C8)</f>
+        <f t="shared" si="0"/>
         <v>59.991500000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>50.006</v>
       </c>
@@ -615,11 +693,41 @@
         <v>50.0015</v>
       </c>
       <c r="D9">
-        <f>SUM(A9:C9)</f>
+        <f t="shared" si="0"/>
         <v>150.0085</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="G11" s="5"/>
+      <c r="H11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>70.008499999999998</v>
       </c>
@@ -635,23 +743,36 @@
         <f>C12-B12</f>
         <v>-4.5499999999947249E-2</v>
       </c>
-      <c r="F12">
+      <c r="G12" s="5"/>
+      <c r="H12" s="4">
         <v>10.0085</v>
       </c>
-      <c r="G12">
+      <c r="I12" s="4">
         <v>20.001000000000001</v>
       </c>
-      <c r="H12">
+      <c r="J12" s="4">
         <v>30.010999999999999</v>
       </c>
-      <c r="I12">
+      <c r="K12" s="4">
         <v>40.0015</v>
       </c>
-      <c r="J12">
+      <c r="L12" s="4">
         <v>50.008000000000003</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M12" s="4">
+        <v>60.000999999999998</v>
+      </c>
+      <c r="N12" s="4">
+        <v>70.007999999999996</v>
+      </c>
+      <c r="O12" s="4">
+        <v>80.001000000000005</v>
+      </c>
+      <c r="P12" s="4">
+        <v>90.006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>19.998999999999999</v>
       </c>
@@ -664,26 +785,41 @@
         <v>200</v>
       </c>
       <c r="D13">
-        <f t="shared" ref="D13:D14" si="1">C13-B13</f>
+        <f t="shared" ref="D13:D14" si="2">C13-B13</f>
         <v>3.7000000000006139E-2</v>
       </c>
-      <c r="F13">
+      <c r="G13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="4">
         <v>9.9990000000000006</v>
       </c>
-      <c r="G13">
+      <c r="I13" s="4">
         <v>20.009499999999999</v>
       </c>
-      <c r="H13">
+      <c r="J13" s="4">
         <v>30.001000000000001</v>
       </c>
-      <c r="I13">
+      <c r="K13" s="4">
         <v>40.005499999999998</v>
       </c>
-      <c r="J13">
-        <v>50.000999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L13" s="4">
+        <v>50.000999999999998</v>
+      </c>
+      <c r="M13" s="4">
+        <v>60.006999999999998</v>
+      </c>
+      <c r="N13" s="4">
+        <v>70.001000000000005</v>
+      </c>
+      <c r="O13" s="4">
+        <v>80.004499999999993</v>
+      </c>
+      <c r="P13" s="4">
+        <v>90.001000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>50.008000000000003</v>
       </c>
@@ -696,453 +832,462 @@
         <v>500</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-3.9999999999906777E-2</v>
       </c>
-      <c r="F14">
+      <c r="G14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="4">
         <v>9.9939999999999998</v>
       </c>
-      <c r="G14">
+      <c r="I14" s="4">
         <v>20.001000000000001</v>
       </c>
-      <c r="H14">
+      <c r="J14" s="4">
         <v>30.008500000000002</v>
       </c>
-      <c r="I14">
+      <c r="K14" s="4">
         <v>40.0015</v>
       </c>
-      <c r="J14">
+      <c r="L14" s="4">
         <v>50.009</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M14" s="4">
+        <v>60.000500000000002</v>
+      </c>
+      <c r="N14" s="4">
+        <v>70.008499999999998</v>
+      </c>
+      <c r="O14" s="4">
+        <v>80.001000000000005</v>
+      </c>
+      <c r="P14" s="4">
+        <v>90.009</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>70.000500000000002</v>
       </c>
-      <c r="F15">
+      <c r="G15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="4">
         <v>9.9990000000000006</v>
       </c>
-      <c r="G15">
+      <c r="I15" s="4">
         <v>20.007999999999999</v>
       </c>
-      <c r="H15">
+      <c r="J15" s="4">
         <v>30.0015</v>
       </c>
-      <c r="I15">
+      <c r="K15" s="4">
         <v>40.008499999999998</v>
       </c>
-      <c r="J15">
-        <v>50.000999999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L15" s="4">
+        <v>50.000999999999998</v>
+      </c>
+      <c r="M15" s="4">
+        <v>60.0105</v>
+      </c>
+      <c r="N15" s="4">
+        <v>70.001000000000005</v>
+      </c>
+      <c r="O15" s="4">
+        <v>80.007499999999993</v>
+      </c>
+      <c r="P15" s="4">
+        <v>90.001000000000005</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>19.994</v>
       </c>
-      <c r="F16">
+      <c r="G16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="4">
         <v>9.9934999999999992</v>
       </c>
-      <c r="G16">
+      <c r="I16" s="4">
         <v>20.001000000000001</v>
       </c>
-      <c r="H16">
+      <c r="J16" s="4">
         <v>30.004999999999999</v>
       </c>
-      <c r="I16">
+      <c r="K16" s="4">
         <v>40.000999999999998</v>
       </c>
-      <c r="J16">
+      <c r="L16" s="4">
         <v>50.0075</v>
       </c>
-      <c r="L16" s="2">
-        <f>100-F22</f>
-        <v>1.5500000000017167E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M16" s="4">
+        <v>60.000999999999998</v>
+      </c>
+      <c r="N16" s="4">
+        <v>70.006</v>
+      </c>
+      <c r="O16" s="4">
+        <v>80.001000000000005</v>
+      </c>
+      <c r="P16" s="4">
+        <v>90.006500000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>50.000999999999998</v>
       </c>
-      <c r="F17">
+      <c r="G17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="4">
         <v>9.9990000000000006</v>
       </c>
-      <c r="G17">
+      <c r="I17" s="4">
         <v>20.005500000000001</v>
       </c>
-      <c r="H17">
+      <c r="J17" s="4">
         <v>30.001000000000001</v>
       </c>
-      <c r="I17">
+      <c r="K17" s="4">
         <v>40.003999999999998</v>
       </c>
-      <c r="J17">
-        <v>50.000999999999998</v>
-      </c>
-      <c r="L17" s="3">
-        <f>200-G22</f>
-        <v>-4.4999999999987494E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L17" s="4">
+        <v>50.000999999999998</v>
+      </c>
+      <c r="M17" s="4">
+        <v>60.008499999999998</v>
+      </c>
+      <c r="N17" s="4">
+        <v>70.001000000000005</v>
+      </c>
+      <c r="O17" s="4">
+        <v>80.005499999999998</v>
+      </c>
+      <c r="P17" s="4">
+        <v>90.001000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>70.009500000000003</v>
       </c>
-      <c r="F18">
+      <c r="G18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="4">
         <v>9.9945000000000004</v>
       </c>
-      <c r="G18">
+      <c r="I18" s="4">
         <v>20.001000000000001</v>
       </c>
-      <c r="H18">
+      <c r="J18" s="4">
         <v>30.007999999999999</v>
       </c>
-      <c r="I18">
+      <c r="K18" s="4">
         <v>40.0015</v>
       </c>
-      <c r="J18">
-        <v>50.000999999999998</v>
-      </c>
-      <c r="L18" s="2">
-        <f>300-H22</f>
-        <v>-4.7499999999956799E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L18" s="4">
+        <v>50.000999999999998</v>
+      </c>
+      <c r="M18" s="4">
+        <v>60.003999999999998</v>
+      </c>
+      <c r="N18" s="4">
+        <v>70.001000000000005</v>
+      </c>
+      <c r="O18" s="4">
+        <v>80.007000000000005</v>
+      </c>
+      <c r="P18" s="4">
+        <v>90.001000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>19.998999999999999</v>
       </c>
-      <c r="F19">
+      <c r="G19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="4">
         <v>9.9990000000000006</v>
       </c>
-      <c r="G19">
+      <c r="I19" s="4">
         <v>20.009499999999999</v>
       </c>
-      <c r="H19">
+      <c r="J19" s="4">
         <v>30.001000000000001</v>
       </c>
-      <c r="I19">
+      <c r="K19" s="4">
         <v>40.0045</v>
       </c>
-      <c r="J19">
-        <v>50.000999999999998</v>
-      </c>
-      <c r="L19" s="2">
-        <f>400-I22</f>
-        <v>-3.4499999999979991E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L19" s="4">
+        <v>50.000999999999998</v>
+      </c>
+      <c r="M19" s="4">
+        <v>60.008499999999998</v>
+      </c>
+      <c r="N19" s="4">
+        <v>70.001000000000005</v>
+      </c>
+      <c r="O19" s="4">
+        <v>80.001000000000005</v>
+      </c>
+      <c r="P19" s="4">
+        <v>90.004999999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>50.006500000000003</v>
       </c>
-      <c r="F20">
+      <c r="G20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="4">
         <v>9.9990000000000006</v>
       </c>
-      <c r="G20">
+      <c r="I20" s="4">
         <v>20.001000000000001</v>
       </c>
-      <c r="H20">
+      <c r="J20" s="4">
         <v>30.009499999999999</v>
       </c>
-      <c r="I20">
+      <c r="K20" s="4">
         <v>40.000999999999998</v>
       </c>
-      <c r="J20">
+      <c r="L20" s="4">
         <v>50.006999999999998</v>
       </c>
-      <c r="L20" s="2">
-        <f>500-J22</f>
-        <v>-3.7499999999909051E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="M20" s="4">
+        <v>60.000999999999998</v>
+      </c>
+      <c r="N20" s="4">
+        <v>70.006</v>
+      </c>
+      <c r="O20" s="4">
+        <v>80.001000000000005</v>
+      </c>
+      <c r="P20" s="4">
+        <v>90.004000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>70.001000000000005</v>
       </c>
-      <c r="F21">
+      <c r="G21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="4">
         <v>9.9990000000000006</v>
       </c>
-      <c r="G21">
+      <c r="I21" s="4">
         <v>20.0075</v>
       </c>
-      <c r="H21">
+      <c r="J21" s="4">
         <v>30.001000000000001</v>
       </c>
-      <c r="I21">
+      <c r="K21" s="4">
         <v>40.005499999999998</v>
       </c>
-      <c r="J21">
-        <v>50.000999999999998</v>
-      </c>
-      <c r="L21" s="3">
-        <f>600-F34</f>
-        <v>-4.7000000000025466E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="L21" s="4">
+        <v>50.000999999999998</v>
+      </c>
+      <c r="M21" s="4">
+        <v>60.005000000000003</v>
+      </c>
+      <c r="N21" s="4">
+        <v>70.001000000000005</v>
+      </c>
+      <c r="O21" s="4">
+        <v>80.007499999999993</v>
+      </c>
+      <c r="P21" s="4">
+        <v>90.001000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>19.992000000000001</v>
       </c>
-      <c r="F22">
-        <f>SUM(F12:F21)</f>
+      <c r="G22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="4">
+        <f>SUM(H12:H21)</f>
         <v>99.984499999999983</v>
       </c>
-      <c r="G22">
-        <f t="shared" ref="G22:J22" si="2">SUM(G12:G21)</f>
+      <c r="I22" s="4">
+        <f t="shared" ref="I22:L22" si="3">SUM(I12:I21)</f>
         <v>200.04499999999999</v>
       </c>
-      <c r="H22">
-        <f t="shared" si="2"/>
+      <c r="J22" s="4">
+        <f t="shared" si="3"/>
         <v>300.04749999999996</v>
       </c>
-      <c r="I22">
-        <f t="shared" si="2"/>
+      <c r="K22" s="4">
+        <f t="shared" si="3"/>
         <v>400.03449999999998</v>
       </c>
-      <c r="J22">
-        <f t="shared" si="2"/>
+      <c r="L22" s="4">
+        <f t="shared" si="3"/>
         <v>500.03749999999991</v>
       </c>
-      <c r="L22" s="2">
-        <f>700-G34</f>
+      <c r="M22" s="4">
+        <f>SUM(M12:M21)</f>
+        <v>600.04700000000003</v>
+      </c>
+      <c r="N22" s="4">
+        <f t="shared" ref="N22:P22" si="4">SUM(N12:N21)</f>
+        <v>700.03449999999987</v>
+      </c>
+      <c r="O22" s="4">
+        <f t="shared" si="4"/>
+        <v>800.03699999999981</v>
+      </c>
+      <c r="P22" s="4">
+        <f t="shared" si="4"/>
+        <v>900.03550000000007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A23">
+        <v>50.000999999999998</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="2">
+        <f>100-H22</f>
+        <v>1.5500000000017167E-2</v>
+      </c>
+      <c r="I23" s="3">
+        <f>200-I22</f>
+        <v>-4.4999999999987494E-2</v>
+      </c>
+      <c r="J23" s="2">
+        <f>300-J22</f>
+        <v>-4.7499999999956799E-2</v>
+      </c>
+      <c r="K23" s="2">
+        <f>400-K22</f>
+        <v>-3.4499999999979991E-2</v>
+      </c>
+      <c r="L23" s="2">
+        <f>500-L22</f>
+        <v>-3.7499999999909051E-2</v>
+      </c>
+      <c r="M23" s="3">
+        <f>600-M22</f>
+        <v>-4.7000000000025466E-2</v>
+      </c>
+      <c r="N23" s="2">
+        <f>700-N22</f>
         <v>-3.4499999999866304E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A23">
-        <v>50.000999999999998</v>
-      </c>
-      <c r="L23" s="3">
-        <f>800-H34</f>
+      <c r="O23" s="3">
+        <f>800-O22</f>
         <v>-3.6999999999807187E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="P23" s="2">
+        <f>900-P22</f>
+        <v>-3.5500000000070031E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>70.010000000000005</v>
       </c>
-      <c r="F24">
-        <v>60.000999999999998</v>
-      </c>
-      <c r="G24">
-        <v>70.007999999999996</v>
-      </c>
-      <c r="H24">
-        <v>80.001000000000005</v>
-      </c>
-      <c r="I24">
-        <v>90.006</v>
-      </c>
-      <c r="L24" s="2">
-        <f>900-I34</f>
-        <v>-3.5500000000070031E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>19.998999999999999</v>
       </c>
-      <c r="F25">
-        <v>60.006999999999998</v>
-      </c>
-      <c r="G25">
-        <v>70.001000000000005</v>
-      </c>
-      <c r="H25">
-        <v>80.004499999999993</v>
-      </c>
-      <c r="I25">
-        <v>90.001000000000005</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>50.0075</v>
       </c>
-      <c r="F26">
-        <v>60.000500000000002</v>
-      </c>
-      <c r="G26">
-        <v>70.008499999999998</v>
-      </c>
-      <c r="H26">
-        <v>80.001000000000005</v>
-      </c>
-      <c r="I26">
-        <v>90.009</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>70.001000000000005</v>
       </c>
-      <c r="F27">
-        <v>60.0105</v>
-      </c>
-      <c r="G27">
-        <v>70.001000000000005</v>
-      </c>
-      <c r="H27">
-        <v>80.007499999999993</v>
-      </c>
-      <c r="I27">
-        <v>90.001000000000005</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>19.9955</v>
       </c>
-      <c r="F28">
-        <v>60.000999999999998</v>
-      </c>
-      <c r="G28">
-        <v>70.006</v>
-      </c>
-      <c r="H28">
-        <v>80.001000000000005</v>
-      </c>
-      <c r="I28">
-        <v>90.006500000000003</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>50.000999999999998</v>
       </c>
-      <c r="F29">
-        <v>60.008499999999998</v>
-      </c>
-      <c r="G29">
-        <v>70.001000000000005</v>
-      </c>
-      <c r="H29">
-        <v>80.005499999999998</v>
-      </c>
-      <c r="I29">
-        <v>90.001000000000005</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>70.008499999999998</v>
       </c>
-      <c r="F30">
-        <v>60.003999999999998</v>
-      </c>
-      <c r="G30">
-        <v>70.001000000000005</v>
-      </c>
-      <c r="H30">
-        <v>80.007000000000005</v>
-      </c>
-      <c r="I30">
-        <v>90.001000000000005</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>19.999500000000001</v>
       </c>
-      <c r="F31">
-        <v>60.008499999999998</v>
-      </c>
-      <c r="G31">
-        <v>70.001000000000005</v>
-      </c>
-      <c r="H31">
-        <v>80.001000000000005</v>
-      </c>
-      <c r="I31">
-        <v>90.004999999999995</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>50.0075</v>
       </c>
-      <c r="F32">
-        <v>60.000999999999998</v>
-      </c>
-      <c r="G32">
-        <v>70.006</v>
-      </c>
-      <c r="H32">
-        <v>80.001000000000005</v>
-      </c>
-      <c r="I32">
-        <v>90.004000000000005</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>70.001000000000005</v>
       </c>
-      <c r="F33">
-        <v>60.005000000000003</v>
-      </c>
-      <c r="G33">
-        <v>70.001000000000005</v>
-      </c>
-      <c r="H33">
-        <v>80.007499999999993</v>
-      </c>
-      <c r="I33">
-        <v>90.001000000000005</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>19.994</v>
       </c>
-      <c r="F34">
-        <f>SUM(F24:F33)</f>
-        <v>600.04700000000003</v>
-      </c>
-      <c r="G34">
-        <f t="shared" ref="G34:I34" si="3">SUM(G24:G33)</f>
-        <v>700.03449999999987</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="3"/>
-        <v>800.03699999999981</v>
-      </c>
-      <c r="I34">
-        <f t="shared" si="3"/>
-        <v>900.03550000000007</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>50.000999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>70.004999999999995</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>19.998999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>50.005499999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>70.000500000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>19.992000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>50.000999999999998</v>
       </c>

</xml_diff>